<commit_message>
some changes updated api documentation
</commit_message>
<xml_diff>
--- a/apidoc.xlsx
+++ b/apidoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/master/Documents/jkwrite/bht/runtime/workspaces/madworkspace_s22/org.dieschnittstelle.mobile.samplewebapi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFE0043-5967-4D40-BDA7-32E38B3EA9AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6927164D-31F7-1544-BB68-82EC81BAE46E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4460" yWindow="500" windowWidth="25600" windowHeight="14800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Opertation</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>/api/users/prepare</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>/api/todos/reset</t>
+  </si>
+  <si>
+    <t>Liegen beim Start der Webanwendung keine Todos vor, werden Todos erstellt, die den Rahmenbedingungen für die Abnahme des Semesterprojekts der MAD Lehrveranstaltung  genügen. Die reset Operation stellt diesen Zustand im laufenden Betrieb wieder her.</t>
   </si>
 </sst>
 </file>
@@ -175,10 +184,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -522,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,16 +658,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -663,13 +672,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -678,30 +687,57 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
+  <mergeCells count="3">
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>